<commit_message>
Using XLSX for config/report
</commit_message>
<xml_diff>
--- a/config/ocr-fix-gift-from.xlsx
+++ b/config/ocr-fix-gift-from.xlsx
@@ -20,16 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">OCR</t>
   </si>
   <si>
     <t xml:space="preserve">FIX</t>
   </si>
-  <si>
-    <t xml:space="preserve">[Player Unknown]</t>
-  </si>
 </sst>
 </file>
 
@@ -43,6 +40,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -64,6 +62,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,12 +107,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -240,31 +243,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>